<commit_message>
Bugs con empresas solucionados
</commit_message>
<xml_diff>
--- a/Enterprises.xlsx
+++ b/Enterprises.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Razon Social</t>
   </si>
@@ -45,6 +45,21 @@
   </si>
   <si>
     <t>over@over.com</t>
+  </si>
+  <si>
+    <t>Motiviator</t>
+  </si>
+  <si>
+    <t>MOTIVIATOR</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>terreneitor</t>
+  </si>
+  <si>
+    <t>motiviator@motiviator.com</t>
   </si>
 </sst>
 </file>
@@ -89,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -135,6 +150,26 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Se hace funcional todos los botones, se validan entradas de datos y se agrega la pestaña de planes en empresas
</commit_message>
<xml_diff>
--- a/Enterprises.xlsx
+++ b/Enterprises.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Razon Social</t>
   </si>
@@ -29,37 +29,28 @@
     <t>E-Mail</t>
   </si>
   <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
     <t>Id</t>
   </si>
   <si>
     <t>Over</t>
   </si>
   <si>
-    <t>OverUser</t>
+    <t>900542632-5</t>
   </si>
   <si>
-    <t>900652854-1</t>
-  </si>
-  <si>
-    <t>over1234</t>
+    <t>12345678</t>
   </si>
   <si>
     <t>over@over.com</t>
   </si>
   <si>
-    <t>Motiviator</t>
+    <t>N/A</t>
   </si>
   <si>
-    <t>MOTIVIATOR</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>terreneitor</t>
-  </si>
-  <si>
-    <t>motiviator@motiviator.com</t>
+    <t>Empresa de turismo dedicada a la exportacion de niños y niñas al extrajero con fines de lucro y esclavismo</t>
   </si>
 </sst>
 </file>
@@ -104,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -129,10 +120,13 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -146,28 +140,11 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2.0</v>
+      <c r="G2" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se arreglan la mayoria de bugs
</commit_message>
<xml_diff>
--- a/Enterprises.xlsx
+++ b/Enterprises.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Razon Social</t>
   </si>
@@ -51,6 +51,33 @@
   </si>
   <si>
     <t>Empresa de turismo dedicada a la exportacion de niños y niñas al extrajero con fines de lucro y esclavismo</t>
+  </si>
+  <si>
+    <t>707Air</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>9006568569</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>air@air.com</t>
+  </si>
+  <si>
+    <t>nueva empresa</t>
+  </si>
+  <si>
+    <t>esto</t>
+  </si>
+  <si>
+    <t>6454654654</t>
+  </si>
+  <si>
+    <t>descripcion</t>
   </si>
 </sst>
 </file>
@@ -95,7 +122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -147,6 +174,29 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>